<commit_message>
gitignore was dropping segmentmap.csv
</commit_message>
<xml_diff>
--- a/Documentation/Freesurfer Labels - DTI enabled.xlsx
+++ b/Documentation/Freesurfer Labels - DTI enabled.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="402">
   <si>
     <t xml:space="preserve">FreeSurfer Label</t>
   </si>
@@ -1200,7 +1200,10 @@
     <t xml:space="preserve">Label</t>
   </si>
   <si>
-    <t xml:space="preserve">Asymetry counterpart</t>
+    <t xml:space="preserve">Asymmetry Counterpart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Grey Cunterpart</t>
   </si>
   <si>
     <t xml:space="preserve">Left or Right</t>
@@ -1438,7 +1441,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B14" activeCellId="1" sqref="C2:C42 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3605,7 +3608,7 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="C2:C42 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5755,10 +5758,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F182"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5787,6 +5790,9 @@
       <c r="F1" s="0" t="s">
         <v>395</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="n">
@@ -5796,14 +5802,17 @@
         <f aca="false">VLOOKUP(A2,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Cerebral-White-Matter</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C2" s="9" t="n">
+        <v>41</v>
+      </c>
+      <c r="D2" s="9"/>
       <c r="E2" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F2" s="0" t="str">
+      <c r="F2" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G2" s="0" t="str">
         <f aca="false">VLOOKUP(A2,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left cerebral white matter</v>
       </c>
@@ -5816,14 +5825,17 @@
         <f aca="false">VLOOKUP(A3,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Lateral-Ventricle</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C3" s="9" t="n">
+        <v>43</v>
+      </c>
+      <c r="D3" s="9"/>
       <c r="E3" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F3" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G3" s="0" t="str">
         <f aca="false">VLOOKUP(A3,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lateral ventricle</v>
       </c>
@@ -5836,14 +5848,17 @@
         <f aca="false">VLOOKUP(A4,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Inf-Lat-Vent</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C4" s="9" t="n">
+        <v>44</v>
+      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F4" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G4" s="0" t="str">
         <f aca="false">VLOOKUP(A4,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left inferior lateral ventricle</v>
       </c>
@@ -5857,16 +5872,19 @@
         <v>Left-Cerebellum-White-Matter</v>
       </c>
       <c r="C5" s="9" t="n">
+        <v>46</v>
+      </c>
+      <c r="D5" s="9" t="n">
         <f aca="false">VLOOKUP(A5,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>8</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E5" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F5" s="0" t="str">
+      <c r="F5" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G5" s="0" t="str">
         <f aca="false">VLOOKUP(A5,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left cerebellum white matter</v>
       </c>
@@ -5880,16 +5898,19 @@
         <v>Left-Cerebellum-Cortex</v>
       </c>
       <c r="C6" s="9" t="n">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="n">
         <f aca="false">VLOOKUP(A6,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>7</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F6" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G6" s="0" t="str">
         <f aca="false">VLOOKUP(A6,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left cerebellum cortex</v>
       </c>
@@ -5902,14 +5923,17 @@
         <f aca="false">VLOOKUP(A7,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Thalamus-Proper</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C7" s="9" t="n">
+        <v>49</v>
+      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F7" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G7" s="0" t="str">
         <f aca="false">VLOOKUP(A7,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left thalamus proper</v>
       </c>
@@ -5922,14 +5946,17 @@
         <f aca="false">VLOOKUP(A8,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Caudate</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C8" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" s="9"/>
       <c r="E8" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F8" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G8" s="0" t="str">
         <f aca="false">VLOOKUP(A8,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left caudate</v>
       </c>
@@ -5942,14 +5969,17 @@
         <f aca="false">VLOOKUP(A9,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Putamen</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C9" s="9" t="n">
+        <v>51</v>
+      </c>
+      <c r="D9" s="9"/>
       <c r="E9" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F9" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G9" s="0" t="str">
         <f aca="false">VLOOKUP(A9,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left putamen</v>
       </c>
@@ -5962,14 +5992,17 @@
         <f aca="false">VLOOKUP(A10,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Pallidum</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C10" s="9" t="n">
+        <v>52</v>
+      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F10" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G10" s="0" t="str">
         <f aca="false">VLOOKUP(A10,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pallidum</v>
       </c>
@@ -5983,13 +6016,14 @@
         <v>3rd-Ventricle</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D11" s="9"/>
       <c r="E11" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F11" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G11" s="0" t="str">
         <f aca="false">VLOOKUP(A11,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>third ventricle</v>
       </c>
@@ -6003,13 +6037,14 @@
         <v>4th-Ventricle</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F12" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G12" s="0" t="str">
         <f aca="false">VLOOKUP(A12,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>fourth ventricle</v>
       </c>
@@ -6023,13 +6058,14 @@
         <v>Brain-Stem</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F13" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G13" s="0" t="str">
         <f aca="false">VLOOKUP(A13,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>brain stem</v>
       </c>
@@ -6042,14 +6078,17 @@
         <f aca="false">VLOOKUP(A14,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Hippocampus</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C14" s="9" t="n">
+        <v>53</v>
+      </c>
+      <c r="D14" s="9"/>
       <c r="E14" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F14" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G14" s="0" t="str">
         <f aca="false">VLOOKUP(A14,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left hippocampus</v>
       </c>
@@ -6062,14 +6101,17 @@
         <f aca="false">VLOOKUP(A15,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Amygdala</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C15" s="9" t="n">
+        <v>54</v>
+      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F15" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G15" s="0" t="str">
         <f aca="false">VLOOKUP(A15,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left amygdala</v>
       </c>
@@ -6083,13 +6125,14 @@
         <v>CSF</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F16" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G16" s="0" t="str">
         <f aca="false">VLOOKUP(A16,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>cerebrospinal fluid</v>
       </c>
@@ -6102,14 +6145,17 @@
         <f aca="false">VLOOKUP(A17,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-Accumbens-area</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C17" s="9" t="n">
+        <v>58</v>
+      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F17" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G17" s="0" t="str">
         <f aca="false">VLOOKUP(A17,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left accumbens area</v>
       </c>
@@ -6122,14 +6168,17 @@
         <f aca="false">VLOOKUP(A18,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-VentralDC</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C18" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F18" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G18" s="0" t="str">
         <f aca="false">VLOOKUP(A18,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left ventral diencephalon</v>
       </c>
@@ -6142,14 +6191,17 @@
         <f aca="false">VLOOKUP(A19,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-vessel</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C19" s="9" t="n">
+        <v>62</v>
+      </c>
+      <c r="D19" s="9"/>
       <c r="E19" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F19" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G19" s="0" t="str">
         <f aca="false">VLOOKUP(A19,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left vessel</v>
       </c>
@@ -6162,14 +6214,17 @@
         <f aca="false">VLOOKUP(A20,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-choroid-plexus</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C20" s="9" t="n">
+        <v>63</v>
+      </c>
+      <c r="D20" s="9"/>
       <c r="E20" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F20" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G20" s="0" t="str">
         <f aca="false">VLOOKUP(A20,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left choroid plexus</v>
       </c>
@@ -6182,14 +6237,17 @@
         <f aca="false">VLOOKUP(A21,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Cerebral-White-Matter</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="0" t="s">
-        <v>399</v>
-      </c>
+      <c r="C21" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F21" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G21" s="0" t="str">
         <f aca="false">VLOOKUP(A21,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right cerebral white matter</v>
       </c>
@@ -6202,14 +6260,17 @@
         <f aca="false">VLOOKUP(A22,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Lateral-Ventricle</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="0" t="s">
+      <c r="C22" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F22" s="0" t="str">
+      <c r="G22" s="0" t="str">
         <f aca="false">VLOOKUP(A22,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lateral ventricle</v>
       </c>
@@ -6222,14 +6283,17 @@
         <f aca="false">VLOOKUP(A23,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Inf-Lat-Vent</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="0" t="s">
+      <c r="C23" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E23" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F23" s="0" t="str">
+      <c r="G23" s="0" t="str">
         <f aca="false">VLOOKUP(A23,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right inferior lateral ventricle</v>
       </c>
@@ -6243,16 +6307,19 @@
         <v>Right-Cerebellum-White-Matter</v>
       </c>
       <c r="C24" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D24" s="9" t="n">
         <f aca="false">VLOOKUP(A24,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>47</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E24" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F24" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G24" s="0" t="str">
         <f aca="false">VLOOKUP(A24,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right cerebellum white matter</v>
       </c>
@@ -6266,16 +6333,19 @@
         <v>Right-Cerebellum-Cortex</v>
       </c>
       <c r="C25" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D25" s="9" t="n">
         <f aca="false">VLOOKUP(A25,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>46</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F25" s="0" t="str">
+      <c r="G25" s="0" t="str">
         <f aca="false">VLOOKUP(A25,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right cerebellum cortex</v>
       </c>
@@ -6288,14 +6358,17 @@
         <f aca="false">VLOOKUP(A26,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Thalamus-Proper</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="0" t="s">
+      <c r="C26" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F26" s="0" t="str">
+      <c r="G26" s="0" t="str">
         <f aca="false">VLOOKUP(A26,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right thalamus proper</v>
       </c>
@@ -6308,14 +6381,17 @@
         <f aca="false">VLOOKUP(A27,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Caudate</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="0" t="s">
+      <c r="C27" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F27" s="0" t="str">
+      <c r="G27" s="0" t="str">
         <f aca="false">VLOOKUP(A27,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right caudate</v>
       </c>
@@ -6328,14 +6404,17 @@
         <f aca="false">VLOOKUP(A28,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Putamen</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="0" t="s">
+      <c r="C28" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F28" s="0" t="str">
+      <c r="G28" s="0" t="str">
         <f aca="false">VLOOKUP(A28,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right putamen</v>
       </c>
@@ -6348,14 +6427,17 @@
         <f aca="false">VLOOKUP(A29,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Pallidum</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="0" t="s">
+      <c r="C29" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F29" s="0" t="str">
+      <c r="G29" s="0" t="str">
         <f aca="false">VLOOKUP(A29,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pallidum</v>
       </c>
@@ -6368,14 +6450,17 @@
         <f aca="false">VLOOKUP(A30,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Hippocampus</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="0" t="s">
+      <c r="C30" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F30" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F30" s="0" t="str">
+      <c r="G30" s="0" t="str">
         <f aca="false">VLOOKUP(A30,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right hippocampus</v>
       </c>
@@ -6388,14 +6473,17 @@
         <f aca="false">VLOOKUP(A31,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Amygdala</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="0" t="s">
+      <c r="C31" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F31" s="0" t="str">
+      <c r="G31" s="0" t="str">
         <f aca="false">VLOOKUP(A31,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right amygdala</v>
       </c>
@@ -6408,14 +6496,17 @@
         <f aca="false">VLOOKUP(A32,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-Accumbens-area</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="0" t="s">
+      <c r="C32" s="9" t="n">
+        <v>26</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F32" s="0" t="str">
+      <c r="G32" s="0" t="str">
         <f aca="false">VLOOKUP(A32,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right accumbens area</v>
       </c>
@@ -6428,14 +6519,17 @@
         <f aca="false">VLOOKUP(A33,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-VentralDC</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="0" t="s">
+      <c r="C33" s="9" t="n">
+        <v>28</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F33" s="0" t="str">
+      <c r="G33" s="0" t="str">
         <f aca="false">VLOOKUP(A33,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right ventral diencephalon</v>
       </c>
@@ -6448,14 +6542,17 @@
         <f aca="false">VLOOKUP(A34,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-vessel</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="0" t="s">
+      <c r="C34" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F34" s="0" t="str">
+      <c r="G34" s="0" t="str">
         <f aca="false">VLOOKUP(A34,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right vessel</v>
       </c>
@@ -6468,14 +6565,17 @@
         <f aca="false">VLOOKUP(A35,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-choroid-plexus</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="0" t="s">
+      <c r="C35" s="9" t="n">
+        <v>31</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F35" s="0" t="str">
+      <c r="G35" s="0" t="str">
         <f aca="false">VLOOKUP(A35,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right choroid plexus</v>
       </c>
@@ -6489,13 +6589,14 @@
         <v>WM-hypointensities</v>
       </c>
       <c r="C36" s="9"/>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F36" s="0" t="str">
+      <c r="G36" s="0" t="str">
         <f aca="false">VLOOKUP(A36,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>white matter hypointensities</v>
       </c>
@@ -6509,13 +6610,14 @@
         <v>Optic-Chiasm</v>
       </c>
       <c r="C37" s="9"/>
-      <c r="D37" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D37" s="9"/>
       <c r="E37" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F37" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G37" s="0" t="str">
         <f aca="false">VLOOKUP(A37,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>optic chiasm</v>
       </c>
@@ -6529,15 +6631,16 @@
         <v>CC_Posterior</v>
       </c>
       <c r="C38" s="9"/>
-      <c r="D38" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D38" s="9"/>
       <c r="E38" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F38" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G38" s="0" t="str">
         <f aca="false">VLOOKUP(A38,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>posterior corpus callosum </v>
+        <v>posterior corpus callosum</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6549,15 +6652,16 @@
         <v>CC_Mid_Posterior</v>
       </c>
       <c r="C39" s="9"/>
-      <c r="D39" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D39" s="9"/>
       <c r="E39" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F39" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G39" s="0" t="str">
         <f aca="false">VLOOKUP(A39,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>mid posterior corpus callosum </v>
+        <v>mid posterior corpus callosum</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6569,15 +6673,16 @@
         <v>CC_Central</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D40" s="9"/>
       <c r="E40" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F40" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G40" s="0" t="str">
         <f aca="false">VLOOKUP(A40,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>central corpus callosum </v>
+        <v>central corpus callosum</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,15 +6694,16 @@
         <v>CC_Mid_Anterior</v>
       </c>
       <c r="C41" s="9"/>
-      <c r="D41" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D41" s="9"/>
       <c r="E41" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F41" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G41" s="0" t="str">
         <f aca="false">VLOOKUP(A41,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>mid anterior corpus callosum </v>
+        <v>mid anterior corpus callosum</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6609,15 +6715,16 @@
         <v>CC_Anterior</v>
       </c>
       <c r="C42" s="9"/>
-      <c r="D42" s="0" t="s">
-        <v>398</v>
-      </c>
+      <c r="D42" s="9"/>
       <c r="E42" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F42" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="G42" s="0" t="str">
         <f aca="false">VLOOKUP(A42,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>anterior corpus callosum </v>
+        <v>anterior corpus callosum</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6628,16 +6735,19 @@
         <f aca="false">VLOOKUP(A43,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-unknown</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C43" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D43" s="9"/>
       <c r="E43" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F43" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G43" s="0" t="str">
         <f aca="false">VLOOKUP(A43,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>unknown left hemisphere grey matter </v>
+        <v>unknown left hemisphere grey matter</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6648,17 +6758,21 @@
         <f aca="false">VLOOKUP(A44,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-bankssts</v>
       </c>
-      <c r="C44" s="9" t="n">
+      <c r="C44" s="0" t="n">
+        <f aca="false">A44+1000</f>
+        <v>2001</v>
+      </c>
+      <c r="D44" s="9" t="n">
         <f aca="false">VLOOKUP(A44,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3001</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E44" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F44" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G44" s="0" t="str">
         <f aca="false">VLOOKUP(A44,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left banks of superior temporal sulcus grey matter</v>
       </c>
@@ -6671,19 +6785,23 @@
         <f aca="false">VLOOKUP(A45,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-caudalanteriorcingulate</v>
       </c>
-      <c r="C45" s="9" t="n">
+      <c r="C45" s="0" t="n">
+        <f aca="false">A45+1000</f>
+        <v>2002</v>
+      </c>
+      <c r="D45" s="9" t="n">
         <f aca="false">VLOOKUP(A45,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3002</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E45" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F45" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G45" s="0" t="str">
         <f aca="false">VLOOKUP(A45,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
-        <v>left caudal anterior cingulate grey matter </v>
+        <v>left caudal anterior cingulate grey matter</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6694,17 +6812,21 @@
         <f aca="false">VLOOKUP(A46,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-caudalmiddlefrontal</v>
       </c>
-      <c r="C46" s="9" t="n">
+      <c r="C46" s="0" t="n">
+        <f aca="false">A46+1000</f>
+        <v>2003</v>
+      </c>
+      <c r="D46" s="9" t="n">
         <f aca="false">VLOOKUP(A46,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3003</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E46" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F46" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G46" s="0" t="str">
         <f aca="false">VLOOKUP(A46,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left caudal middle frontal grey matter</v>
       </c>
@@ -6717,17 +6839,21 @@
         <f aca="false">VLOOKUP(A47,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-cuneus</v>
       </c>
-      <c r="C47" s="9" t="n">
+      <c r="C47" s="0" t="n">
+        <f aca="false">A47+1000</f>
+        <v>2005</v>
+      </c>
+      <c r="D47" s="9" t="n">
         <f aca="false">VLOOKUP(A47,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3005</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E47" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F47" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G47" s="0" t="str">
         <f aca="false">VLOOKUP(A47,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left cuneus grey matter</v>
       </c>
@@ -6740,17 +6866,21 @@
         <f aca="false">VLOOKUP(A48,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-entorhinal</v>
       </c>
-      <c r="C48" s="9" t="n">
+      <c r="C48" s="0" t="n">
+        <f aca="false">A48+1000</f>
+        <v>2006</v>
+      </c>
+      <c r="D48" s="9" t="n">
         <f aca="false">VLOOKUP(A48,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3006</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E48" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F48" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G48" s="0" t="str">
         <f aca="false">VLOOKUP(A48,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left entorhinal grey matter</v>
       </c>
@@ -6763,17 +6893,21 @@
         <f aca="false">VLOOKUP(A49,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-fusiform</v>
       </c>
-      <c r="C49" s="9" t="n">
+      <c r="C49" s="0" t="n">
+        <f aca="false">A49+1000</f>
+        <v>2007</v>
+      </c>
+      <c r="D49" s="9" t="n">
         <f aca="false">VLOOKUP(A49,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3007</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E49" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F49" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G49" s="0" t="str">
         <f aca="false">VLOOKUP(A49,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left fusiform grey matter</v>
       </c>
@@ -6786,17 +6920,21 @@
         <f aca="false">VLOOKUP(A50,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-inferiorparietal</v>
       </c>
-      <c r="C50" s="9" t="n">
+      <c r="C50" s="0" t="n">
+        <f aca="false">A50+1000</f>
+        <v>2008</v>
+      </c>
+      <c r="D50" s="9" t="n">
         <f aca="false">VLOOKUP(A50,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3008</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E50" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F50" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G50" s="0" t="str">
         <f aca="false">VLOOKUP(A50,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left inferior parietal grey matter</v>
       </c>
@@ -6809,17 +6947,21 @@
         <f aca="false">VLOOKUP(A51,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-inferiortemporal</v>
       </c>
-      <c r="C51" s="9" t="n">
+      <c r="C51" s="0" t="n">
+        <f aca="false">A51+1000</f>
+        <v>2009</v>
+      </c>
+      <c r="D51" s="9" t="n">
         <f aca="false">VLOOKUP(A51,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3009</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E51" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F51" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G51" s="0" t="str">
         <f aca="false">VLOOKUP(A51,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left inferior temporal grey matter</v>
       </c>
@@ -6832,17 +6974,21 @@
         <f aca="false">VLOOKUP(A52,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-isthmuscingulate</v>
       </c>
-      <c r="C52" s="9" t="n">
+      <c r="C52" s="0" t="n">
+        <f aca="false">A52+1000</f>
+        <v>2010</v>
+      </c>
+      <c r="D52" s="9" t="n">
         <f aca="false">VLOOKUP(A52,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3010</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E52" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F52" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G52" s="0" t="str">
         <f aca="false">VLOOKUP(A52,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left isthmus cingulate grey matter</v>
       </c>
@@ -6855,17 +7001,21 @@
         <f aca="false">VLOOKUP(A53,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-lateraloccipital</v>
       </c>
-      <c r="C53" s="9" t="n">
+      <c r="C53" s="0" t="n">
+        <f aca="false">A53+1000</f>
+        <v>2011</v>
+      </c>
+      <c r="D53" s="9" t="n">
         <f aca="false">VLOOKUP(A53,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3011</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E53" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F53" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G53" s="0" t="str">
         <f aca="false">VLOOKUP(A53,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lateral occipital grey matter</v>
       </c>
@@ -6878,17 +7028,21 @@
         <f aca="false">VLOOKUP(A54,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-lateralorbitofrontal</v>
       </c>
-      <c r="C54" s="9" t="n">
+      <c r="C54" s="0" t="n">
+        <f aca="false">A54+1000</f>
+        <v>2012</v>
+      </c>
+      <c r="D54" s="9" t="n">
         <f aca="false">VLOOKUP(A54,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3012</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E54" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F54" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G54" s="0" t="str">
         <f aca="false">VLOOKUP(A54,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lateral orbitofrontal grey matter</v>
       </c>
@@ -6901,17 +7055,21 @@
         <f aca="false">VLOOKUP(A55,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-lingual</v>
       </c>
-      <c r="C55" s="9" t="n">
+      <c r="C55" s="0" t="n">
+        <f aca="false">A55+1000</f>
+        <v>2013</v>
+      </c>
+      <c r="D55" s="9" t="n">
         <f aca="false">VLOOKUP(A55,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3013</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E55" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F55" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G55" s="0" t="str">
         <f aca="false">VLOOKUP(A55,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lingual grey matter</v>
       </c>
@@ -6924,17 +7082,21 @@
         <f aca="false">VLOOKUP(A56,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-medialorbitofrontal</v>
       </c>
-      <c r="C56" s="9" t="n">
+      <c r="C56" s="0" t="n">
+        <f aca="false">A56+1000</f>
+        <v>2014</v>
+      </c>
+      <c r="D56" s="9" t="n">
         <f aca="false">VLOOKUP(A56,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3014</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E56" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F56" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G56" s="0" t="str">
         <f aca="false">VLOOKUP(A56,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left medial orbitofrontal grey matter</v>
       </c>
@@ -6947,17 +7109,21 @@
         <f aca="false">VLOOKUP(A57,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-middletemporal</v>
       </c>
-      <c r="C57" s="9" t="n">
+      <c r="C57" s="0" t="n">
+        <f aca="false">A57+1000</f>
+        <v>2015</v>
+      </c>
+      <c r="D57" s="9" t="n">
         <f aca="false">VLOOKUP(A57,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3015</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E57" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F57" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G57" s="0" t="str">
         <f aca="false">VLOOKUP(A57,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left middle temporal grey matter</v>
       </c>
@@ -6970,17 +7136,21 @@
         <f aca="false">VLOOKUP(A58,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-parahippocampal</v>
       </c>
-      <c r="C58" s="9" t="n">
+      <c r="C58" s="0" t="n">
+        <f aca="false">A58+1000</f>
+        <v>2016</v>
+      </c>
+      <c r="D58" s="9" t="n">
         <f aca="false">VLOOKUP(A58,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3016</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E58" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F58" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G58" s="0" t="str">
         <f aca="false">VLOOKUP(A58,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left parahippocampal grey matter</v>
       </c>
@@ -6993,17 +7163,21 @@
         <f aca="false">VLOOKUP(A59,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-paracentral</v>
       </c>
-      <c r="C59" s="9" t="n">
+      <c r="C59" s="0" t="n">
+        <f aca="false">A59+1000</f>
+        <v>2017</v>
+      </c>
+      <c r="D59" s="9" t="n">
         <f aca="false">VLOOKUP(A59,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3017</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E59" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F59" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G59" s="0" t="str">
         <f aca="false">VLOOKUP(A59,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left paracentral grey matter</v>
       </c>
@@ -7016,17 +7190,21 @@
         <f aca="false">VLOOKUP(A60,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-parsopercularis</v>
       </c>
-      <c r="C60" s="9" t="n">
+      <c r="C60" s="0" t="n">
+        <f aca="false">A60+1000</f>
+        <v>2018</v>
+      </c>
+      <c r="D60" s="9" t="n">
         <f aca="false">VLOOKUP(A60,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3018</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E60" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F60" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G60" s="0" t="str">
         <f aca="false">VLOOKUP(A60,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pars opercularis grey matter</v>
       </c>
@@ -7039,17 +7217,21 @@
         <f aca="false">VLOOKUP(A61,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-parsorbitalis</v>
       </c>
-      <c r="C61" s="9" t="n">
+      <c r="C61" s="0" t="n">
+        <f aca="false">A61+1000</f>
+        <v>2019</v>
+      </c>
+      <c r="D61" s="9" t="n">
         <f aca="false">VLOOKUP(A61,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3019</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E61" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F61" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G61" s="0" t="str">
         <f aca="false">VLOOKUP(A61,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pars orbitalis grey matter</v>
       </c>
@@ -7062,17 +7244,21 @@
         <f aca="false">VLOOKUP(A62,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-parstriangularis</v>
       </c>
-      <c r="C62" s="9" t="n">
+      <c r="C62" s="0" t="n">
+        <f aca="false">A62+1000</f>
+        <v>2020</v>
+      </c>
+      <c r="D62" s="9" t="n">
         <f aca="false">VLOOKUP(A62,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3020</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E62" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F62" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G62" s="0" t="str">
         <f aca="false">VLOOKUP(A62,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pars triangularis grey matter</v>
       </c>
@@ -7085,17 +7271,21 @@
         <f aca="false">VLOOKUP(A63,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-pericalcarine</v>
       </c>
-      <c r="C63" s="9" t="n">
+      <c r="C63" s="0" t="n">
+        <f aca="false">A63+1000</f>
+        <v>2021</v>
+      </c>
+      <c r="D63" s="9" t="n">
         <f aca="false">VLOOKUP(A63,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3021</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E63" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F63" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G63" s="0" t="str">
         <f aca="false">VLOOKUP(A63,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pericalcarine grey matter</v>
       </c>
@@ -7108,17 +7298,21 @@
         <f aca="false">VLOOKUP(A64,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-postcentral</v>
       </c>
-      <c r="C64" s="9" t="n">
+      <c r="C64" s="0" t="n">
+        <f aca="false">A64+1000</f>
+        <v>2022</v>
+      </c>
+      <c r="D64" s="9" t="n">
         <f aca="false">VLOOKUP(A64,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3022</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E64" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F64" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G64" s="0" t="str">
         <f aca="false">VLOOKUP(A64,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left postcentral grey matter</v>
       </c>
@@ -7131,17 +7325,21 @@
         <f aca="false">VLOOKUP(A65,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-posteriorcingulate</v>
       </c>
-      <c r="C65" s="9" t="n">
+      <c r="C65" s="0" t="n">
+        <f aca="false">A65+1000</f>
+        <v>2023</v>
+      </c>
+      <c r="D65" s="9" t="n">
         <f aca="false">VLOOKUP(A65,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3023</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E65" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F65" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G65" s="0" t="str">
         <f aca="false">VLOOKUP(A65,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left posterior cingulate grey matter</v>
       </c>
@@ -7154,17 +7352,21 @@
         <f aca="false">VLOOKUP(A66,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-precentral</v>
       </c>
-      <c r="C66" s="9" t="n">
+      <c r="C66" s="0" t="n">
+        <f aca="false">A66+1000</f>
+        <v>2024</v>
+      </c>
+      <c r="D66" s="9" t="n">
         <f aca="false">VLOOKUP(A66,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3024</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E66" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F66" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G66" s="0" t="str">
         <f aca="false">VLOOKUP(A66,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left precentral grey matter</v>
       </c>
@@ -7177,17 +7379,21 @@
         <f aca="false">VLOOKUP(A67,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-precuneus</v>
       </c>
-      <c r="C67" s="9" t="n">
+      <c r="C67" s="0" t="n">
+        <f aca="false">A67+1000</f>
+        <v>2025</v>
+      </c>
+      <c r="D67" s="9" t="n">
         <f aca="false">VLOOKUP(A67,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3025</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E67" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F67" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G67" s="0" t="str">
         <f aca="false">VLOOKUP(A67,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left precuneus grey matter</v>
       </c>
@@ -7200,17 +7406,21 @@
         <f aca="false">VLOOKUP(A68,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-rostralanteriorcingulate</v>
       </c>
-      <c r="C68" s="9" t="n">
+      <c r="C68" s="0" t="n">
+        <f aca="false">A68+1000</f>
+        <v>2026</v>
+      </c>
+      <c r="D68" s="9" t="n">
         <f aca="false">VLOOKUP(A68,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3026</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E68" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F68" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G68" s="0" t="str">
         <f aca="false">VLOOKUP(A68,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left rostral anterior cingulate grey matter</v>
       </c>
@@ -7223,17 +7433,21 @@
         <f aca="false">VLOOKUP(A69,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-rostralmiddlefrontal</v>
       </c>
-      <c r="C69" s="9" t="n">
+      <c r="C69" s="0" t="n">
+        <f aca="false">A69+1000</f>
+        <v>2027</v>
+      </c>
+      <c r="D69" s="9" t="n">
         <f aca="false">VLOOKUP(A69,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3027</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E69" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F69" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G69" s="0" t="str">
         <f aca="false">VLOOKUP(A69,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left rostral middle frontal grey matter</v>
       </c>
@@ -7246,17 +7460,21 @@
         <f aca="false">VLOOKUP(A70,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-superiorfrontal</v>
       </c>
-      <c r="C70" s="9" t="n">
+      <c r="C70" s="0" t="n">
+        <f aca="false">A70+1000</f>
+        <v>2028</v>
+      </c>
+      <c r="D70" s="9" t="n">
         <f aca="false">VLOOKUP(A70,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3028</v>
       </c>
-      <c r="D70" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E70" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F70" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G70" s="0" t="str">
         <f aca="false">VLOOKUP(A70,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left superior frontal grey matter</v>
       </c>
@@ -7269,17 +7487,21 @@
         <f aca="false">VLOOKUP(A71,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-superiorparietal</v>
       </c>
-      <c r="C71" s="9" t="n">
+      <c r="C71" s="0" t="n">
+        <f aca="false">A71+1000</f>
+        <v>2029</v>
+      </c>
+      <c r="D71" s="9" t="n">
         <f aca="false">VLOOKUP(A71,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3029</v>
       </c>
-      <c r="D71" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E71" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F71" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G71" s="0" t="str">
         <f aca="false">VLOOKUP(A71,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left superior parietal grey matter</v>
       </c>
@@ -7292,17 +7514,21 @@
         <f aca="false">VLOOKUP(A72,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-superiortemporal</v>
       </c>
-      <c r="C72" s="9" t="n">
+      <c r="C72" s="0" t="n">
+        <f aca="false">A72+1000</f>
+        <v>2030</v>
+      </c>
+      <c r="D72" s="9" t="n">
         <f aca="false">VLOOKUP(A72,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3030</v>
       </c>
-      <c r="D72" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E72" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F72" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G72" s="0" t="str">
         <f aca="false">VLOOKUP(A72,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left superior temporal grey matter</v>
       </c>
@@ -7315,17 +7541,21 @@
         <f aca="false">VLOOKUP(A73,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-supramarginal</v>
       </c>
-      <c r="C73" s="9" t="n">
+      <c r="C73" s="0" t="n">
+        <f aca="false">A73+1000</f>
+        <v>2031</v>
+      </c>
+      <c r="D73" s="9" t="n">
         <f aca="false">VLOOKUP(A73,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3031</v>
       </c>
-      <c r="D73" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E73" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F73" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G73" s="0" t="str">
         <f aca="false">VLOOKUP(A73,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left supramarginal grey matter</v>
       </c>
@@ -7338,17 +7568,21 @@
         <f aca="false">VLOOKUP(A74,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-frontalpole</v>
       </c>
-      <c r="C74" s="9" t="n">
+      <c r="C74" s="0" t="n">
+        <f aca="false">A74+1000</f>
+        <v>2032</v>
+      </c>
+      <c r="D74" s="9" t="n">
         <f aca="false">VLOOKUP(A74,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3032</v>
       </c>
-      <c r="D74" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E74" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F74" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G74" s="0" t="str">
         <f aca="false">VLOOKUP(A74,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left frontal pole grey matter</v>
       </c>
@@ -7361,17 +7595,21 @@
         <f aca="false">VLOOKUP(A75,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-temporalpole</v>
       </c>
-      <c r="C75" s="9" t="n">
+      <c r="C75" s="0" t="n">
+        <f aca="false">A75+1000</f>
+        <v>2033</v>
+      </c>
+      <c r="D75" s="9" t="n">
         <f aca="false">VLOOKUP(A75,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3033</v>
       </c>
-      <c r="D75" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E75" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F75" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G75" s="0" t="str">
         <f aca="false">VLOOKUP(A75,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left temporal pole grey matter</v>
       </c>
@@ -7384,17 +7622,21 @@
         <f aca="false">VLOOKUP(A76,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-transversetemporal</v>
       </c>
-      <c r="C76" s="9" t="n">
+      <c r="C76" s="0" t="n">
+        <f aca="false">A76+1000</f>
+        <v>2034</v>
+      </c>
+      <c r="D76" s="9" t="n">
         <f aca="false">VLOOKUP(A76,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3034</v>
       </c>
-      <c r="D76" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E76" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F76" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G76" s="0" t="str">
         <f aca="false">VLOOKUP(A76,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left transverse temporal grey matter</v>
       </c>
@@ -7407,17 +7649,21 @@
         <f aca="false">VLOOKUP(A77,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-lh-insula</v>
       </c>
-      <c r="C77" s="9" t="n">
+      <c r="C77" s="0" t="n">
+        <f aca="false">A77+1000</f>
+        <v>2035</v>
+      </c>
+      <c r="D77" s="9" t="n">
         <f aca="false">VLOOKUP(A77,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>3035</v>
       </c>
-      <c r="D77" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E77" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="F77" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G77" s="0" t="str">
         <f aca="false">VLOOKUP(A77,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left insula grey matter</v>
       </c>
@@ -7430,14 +7676,18 @@
         <f aca="false">VLOOKUP(A78,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-unknown</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="0" t="s">
-        <v>399</v>
-      </c>
+      <c r="C78" s="0" t="n">
+        <f aca="false">A78-1000</f>
+        <v>1000</v>
+      </c>
+      <c r="D78" s="9"/>
       <c r="E78" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F78" s="0" t="str">
+      <c r="F78" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G78" s="0" t="str">
         <f aca="false">VLOOKUP(A78,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right hemisphere unknown grey matter</v>
       </c>
@@ -7450,17 +7700,21 @@
         <f aca="false">VLOOKUP(A79,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-bankssts</v>
       </c>
-      <c r="C79" s="9" t="n">
+      <c r="C79" s="0" t="n">
+        <f aca="false">A79-1000</f>
+        <v>1001</v>
+      </c>
+      <c r="D79" s="9" t="n">
         <f aca="false">VLOOKUP(A79,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4001</v>
       </c>
-      <c r="D79" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E79" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F79" s="0" t="str">
+      <c r="F79" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G79" s="0" t="str">
         <f aca="false">VLOOKUP(A79,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right banks of superior temporal sulcus grey matter</v>
       </c>
@@ -7473,17 +7727,21 @@
         <f aca="false">VLOOKUP(A80,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-caudalanteriorcingulate</v>
       </c>
-      <c r="C80" s="9" t="n">
+      <c r="C80" s="0" t="n">
+        <f aca="false">A80-1000</f>
+        <v>1002</v>
+      </c>
+      <c r="D80" s="9" t="n">
         <f aca="false">VLOOKUP(A80,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4002</v>
       </c>
-      <c r="D80" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E80" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F80" s="0" t="str">
+      <c r="F80" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G80" s="0" t="str">
         <f aca="false">VLOOKUP(A80,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right caudal anterior cingulate grey matter</v>
       </c>
@@ -7496,17 +7754,21 @@
         <f aca="false">VLOOKUP(A81,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-caudalmiddlefrontal</v>
       </c>
-      <c r="C81" s="9" t="n">
+      <c r="C81" s="0" t="n">
+        <f aca="false">A81-1000</f>
+        <v>1003</v>
+      </c>
+      <c r="D81" s="9" t="n">
         <f aca="false">VLOOKUP(A81,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4003</v>
       </c>
-      <c r="D81" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E81" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F81" s="0" t="str">
+      <c r="F81" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G81" s="0" t="str">
         <f aca="false">VLOOKUP(A81,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right caudal middle frontal grey matter</v>
       </c>
@@ -7519,17 +7781,21 @@
         <f aca="false">VLOOKUP(A82,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-cuneus</v>
       </c>
-      <c r="C82" s="9" t="n">
+      <c r="C82" s="0" t="n">
+        <f aca="false">A82-1000</f>
+        <v>1005</v>
+      </c>
+      <c r="D82" s="9" t="n">
         <f aca="false">VLOOKUP(A82,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4005</v>
       </c>
-      <c r="D82" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E82" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F82" s="0" t="str">
+      <c r="F82" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G82" s="0" t="str">
         <f aca="false">VLOOKUP(A82,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right cuneus grey matter</v>
       </c>
@@ -7542,17 +7808,21 @@
         <f aca="false">VLOOKUP(A83,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-entorhinal</v>
       </c>
-      <c r="C83" s="9" t="n">
+      <c r="C83" s="0" t="n">
+        <f aca="false">A83-1000</f>
+        <v>1006</v>
+      </c>
+      <c r="D83" s="9" t="n">
         <f aca="false">VLOOKUP(A83,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4006</v>
       </c>
-      <c r="D83" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E83" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F83" s="0" t="str">
+      <c r="F83" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G83" s="0" t="str">
         <f aca="false">VLOOKUP(A83,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right entorhinal grey matter</v>
       </c>
@@ -7565,17 +7835,21 @@
         <f aca="false">VLOOKUP(A84,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-fusiform</v>
       </c>
-      <c r="C84" s="9" t="n">
+      <c r="C84" s="0" t="n">
+        <f aca="false">A84-1000</f>
+        <v>1007</v>
+      </c>
+      <c r="D84" s="9" t="n">
         <f aca="false">VLOOKUP(A84,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4007</v>
       </c>
-      <c r="D84" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E84" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F84" s="0" t="str">
+      <c r="F84" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G84" s="0" t="str">
         <f aca="false">VLOOKUP(A84,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right fusiform grey matter</v>
       </c>
@@ -7588,17 +7862,21 @@
         <f aca="false">VLOOKUP(A85,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-inferiorparietal</v>
       </c>
-      <c r="C85" s="9" t="n">
+      <c r="C85" s="0" t="n">
+        <f aca="false">A85-1000</f>
+        <v>1008</v>
+      </c>
+      <c r="D85" s="9" t="n">
         <f aca="false">VLOOKUP(A85,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4008</v>
       </c>
-      <c r="D85" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E85" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F85" s="0" t="str">
+      <c r="F85" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G85" s="0" t="str">
         <f aca="false">VLOOKUP(A85,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right inferior parietal grey matter</v>
       </c>
@@ -7611,17 +7889,21 @@
         <f aca="false">VLOOKUP(A86,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-inferiortemporal</v>
       </c>
-      <c r="C86" s="9" t="n">
+      <c r="C86" s="0" t="n">
+        <f aca="false">A86-1000</f>
+        <v>1009</v>
+      </c>
+      <c r="D86" s="9" t="n">
         <f aca="false">VLOOKUP(A86,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4009</v>
       </c>
-      <c r="D86" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E86" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F86" s="0" t="str">
+      <c r="F86" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G86" s="0" t="str">
         <f aca="false">VLOOKUP(A86,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right inferior temporal grey matter</v>
       </c>
@@ -7634,17 +7916,21 @@
         <f aca="false">VLOOKUP(A87,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-isthmuscingulate</v>
       </c>
-      <c r="C87" s="9" t="n">
+      <c r="C87" s="0" t="n">
+        <f aca="false">A87-1000</f>
+        <v>1010</v>
+      </c>
+      <c r="D87" s="9" t="n">
         <f aca="false">VLOOKUP(A87,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4010</v>
       </c>
-      <c r="D87" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E87" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F87" s="0" t="str">
+      <c r="F87" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G87" s="0" t="str">
         <f aca="false">VLOOKUP(A87,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right isthmus cingulate grey matter</v>
       </c>
@@ -7657,17 +7943,21 @@
         <f aca="false">VLOOKUP(A88,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-lateraloccipital</v>
       </c>
-      <c r="C88" s="9" t="n">
+      <c r="C88" s="0" t="n">
+        <f aca="false">A88-1000</f>
+        <v>1011</v>
+      </c>
+      <c r="D88" s="9" t="n">
         <f aca="false">VLOOKUP(A88,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4011</v>
       </c>
-      <c r="D88" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E88" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F88" s="0" t="str">
+      <c r="F88" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G88" s="0" t="str">
         <f aca="false">VLOOKUP(A88,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lateral occipital grey matter</v>
       </c>
@@ -7680,17 +7970,21 @@
         <f aca="false">VLOOKUP(A89,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-lateralorbitofrontal</v>
       </c>
-      <c r="C89" s="9" t="n">
+      <c r="C89" s="0" t="n">
+        <f aca="false">A89-1000</f>
+        <v>1012</v>
+      </c>
+      <c r="D89" s="9" t="n">
         <f aca="false">VLOOKUP(A89,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4012</v>
       </c>
-      <c r="D89" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E89" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F89" s="0" t="str">
+      <c r="F89" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G89" s="0" t="str">
         <f aca="false">VLOOKUP(A89,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lateral orbitofrontal grey matter</v>
       </c>
@@ -7703,17 +7997,21 @@
         <f aca="false">VLOOKUP(A90,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-lingual</v>
       </c>
-      <c r="C90" s="9" t="n">
+      <c r="C90" s="0" t="n">
+        <f aca="false">A90-1000</f>
+        <v>1013</v>
+      </c>
+      <c r="D90" s="9" t="n">
         <f aca="false">VLOOKUP(A90,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4013</v>
       </c>
-      <c r="D90" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E90" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F90" s="0" t="str">
+      <c r="F90" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G90" s="0" t="str">
         <f aca="false">VLOOKUP(A90,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lingual grey matter</v>
       </c>
@@ -7726,17 +8024,21 @@
         <f aca="false">VLOOKUP(A91,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-medialorbitofrontal</v>
       </c>
-      <c r="C91" s="9" t="n">
+      <c r="C91" s="0" t="n">
+        <f aca="false">A91-1000</f>
+        <v>1014</v>
+      </c>
+      <c r="D91" s="9" t="n">
         <f aca="false">VLOOKUP(A91,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4014</v>
       </c>
-      <c r="D91" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E91" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F91" s="0" t="str">
+      <c r="F91" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G91" s="0" t="str">
         <f aca="false">VLOOKUP(A91,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right medial orbitofrontal grey matter</v>
       </c>
@@ -7749,17 +8051,21 @@
         <f aca="false">VLOOKUP(A92,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-middletemporal</v>
       </c>
-      <c r="C92" s="9" t="n">
+      <c r="C92" s="0" t="n">
+        <f aca="false">A92-1000</f>
+        <v>1015</v>
+      </c>
+      <c r="D92" s="9" t="n">
         <f aca="false">VLOOKUP(A92,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4015</v>
       </c>
-      <c r="D92" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E92" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F92" s="0" t="str">
+      <c r="F92" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G92" s="0" t="str">
         <f aca="false">VLOOKUP(A92,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right middle temporal grey matter</v>
       </c>
@@ -7772,17 +8078,21 @@
         <f aca="false">VLOOKUP(A93,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-parahippocampal</v>
       </c>
-      <c r="C93" s="9" t="n">
+      <c r="C93" s="0" t="n">
+        <f aca="false">A93-1000</f>
+        <v>1016</v>
+      </c>
+      <c r="D93" s="9" t="n">
         <f aca="false">VLOOKUP(A93,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4016</v>
       </c>
-      <c r="D93" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E93" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F93" s="0" t="str">
+      <c r="F93" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G93" s="0" t="str">
         <f aca="false">VLOOKUP(A93,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right parahippocampal grey matter</v>
       </c>
@@ -7795,17 +8105,21 @@
         <f aca="false">VLOOKUP(A94,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-paracentral</v>
       </c>
-      <c r="C94" s="9" t="n">
+      <c r="C94" s="0" t="n">
+        <f aca="false">A94-1000</f>
+        <v>1017</v>
+      </c>
+      <c r="D94" s="9" t="n">
         <f aca="false">VLOOKUP(A94,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4017</v>
       </c>
-      <c r="D94" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E94" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F94" s="0" t="str">
+      <c r="F94" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G94" s="0" t="str">
         <f aca="false">VLOOKUP(A94,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right paracentral grey matter</v>
       </c>
@@ -7818,17 +8132,21 @@
         <f aca="false">VLOOKUP(A95,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-parsopercularis</v>
       </c>
-      <c r="C95" s="9" t="n">
+      <c r="C95" s="0" t="n">
+        <f aca="false">A95-1000</f>
+        <v>1018</v>
+      </c>
+      <c r="D95" s="9" t="n">
         <f aca="false">VLOOKUP(A95,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4018</v>
       </c>
-      <c r="D95" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E95" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F95" s="0" t="str">
+      <c r="F95" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G95" s="0" t="str">
         <f aca="false">VLOOKUP(A95,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pars opercularis grey matter</v>
       </c>
@@ -7841,17 +8159,21 @@
         <f aca="false">VLOOKUP(A96,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-parsorbitalis</v>
       </c>
-      <c r="C96" s="9" t="n">
+      <c r="C96" s="0" t="n">
+        <f aca="false">A96-1000</f>
+        <v>1019</v>
+      </c>
+      <c r="D96" s="9" t="n">
         <f aca="false">VLOOKUP(A96,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4019</v>
       </c>
-      <c r="D96" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E96" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F96" s="0" t="str">
+      <c r="F96" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G96" s="0" t="str">
         <f aca="false">VLOOKUP(A96,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pars orbitalis grey matter</v>
       </c>
@@ -7864,17 +8186,21 @@
         <f aca="false">VLOOKUP(A97,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-parstriangularis</v>
       </c>
-      <c r="C97" s="9" t="n">
+      <c r="C97" s="0" t="n">
+        <f aca="false">A97-1000</f>
+        <v>1020</v>
+      </c>
+      <c r="D97" s="9" t="n">
         <f aca="false">VLOOKUP(A97,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4020</v>
       </c>
-      <c r="D97" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E97" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F97" s="0" t="str">
+      <c r="F97" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G97" s="0" t="str">
         <f aca="false">VLOOKUP(A97,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pars triangularis grey matter</v>
       </c>
@@ -7887,17 +8213,21 @@
         <f aca="false">VLOOKUP(A98,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-pericalcarine</v>
       </c>
-      <c r="C98" s="9" t="n">
+      <c r="C98" s="0" t="n">
+        <f aca="false">A98-1000</f>
+        <v>1021</v>
+      </c>
+      <c r="D98" s="9" t="n">
         <f aca="false">VLOOKUP(A98,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4021</v>
       </c>
-      <c r="D98" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E98" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F98" s="0" t="str">
+      <c r="F98" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G98" s="0" t="str">
         <f aca="false">VLOOKUP(A98,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pericalcarine grey matter</v>
       </c>
@@ -7910,17 +8240,21 @@
         <f aca="false">VLOOKUP(A99,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-postcentral</v>
       </c>
-      <c r="C99" s="9" t="n">
+      <c r="C99" s="0" t="n">
+        <f aca="false">A99-1000</f>
+        <v>1022</v>
+      </c>
+      <c r="D99" s="9" t="n">
         <f aca="false">VLOOKUP(A99,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4022</v>
       </c>
-      <c r="D99" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E99" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F99" s="0" t="str">
+      <c r="F99" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G99" s="0" t="str">
         <f aca="false">VLOOKUP(A99,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right postcentral grey matter</v>
       </c>
@@ -7933,17 +8267,21 @@
         <f aca="false">VLOOKUP(A100,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-posteriorcingulate</v>
       </c>
-      <c r="C100" s="9" t="n">
+      <c r="C100" s="0" t="n">
+        <f aca="false">A100-1000</f>
+        <v>1023</v>
+      </c>
+      <c r="D100" s="9" t="n">
         <f aca="false">VLOOKUP(A100,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4023</v>
       </c>
-      <c r="D100" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E100" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F100" s="0" t="str">
+      <c r="F100" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G100" s="0" t="str">
         <f aca="false">VLOOKUP(A100,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right posterior cingulate grey matter</v>
       </c>
@@ -7956,17 +8294,21 @@
         <f aca="false">VLOOKUP(A101,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-precentral</v>
       </c>
-      <c r="C101" s="9" t="n">
+      <c r="C101" s="0" t="n">
+        <f aca="false">A101-1000</f>
+        <v>1024</v>
+      </c>
+      <c r="D101" s="9" t="n">
         <f aca="false">VLOOKUP(A101,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4024</v>
       </c>
-      <c r="D101" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E101" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F101" s="0" t="str">
+      <c r="F101" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G101" s="0" t="str">
         <f aca="false">VLOOKUP(A101,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right precentral grey matter</v>
       </c>
@@ -7979,17 +8321,21 @@
         <f aca="false">VLOOKUP(A102,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-precuneus</v>
       </c>
-      <c r="C102" s="9" t="n">
+      <c r="C102" s="0" t="n">
+        <f aca="false">A102-1000</f>
+        <v>1025</v>
+      </c>
+      <c r="D102" s="9" t="n">
         <f aca="false">VLOOKUP(A102,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4025</v>
       </c>
-      <c r="D102" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E102" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F102" s="0" t="str">
+      <c r="F102" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G102" s="0" t="str">
         <f aca="false">VLOOKUP(A102,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right precuneus grey matter</v>
       </c>
@@ -8002,17 +8348,21 @@
         <f aca="false">VLOOKUP(A103,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-rostralanteriorcingulate</v>
       </c>
-      <c r="C103" s="9" t="n">
+      <c r="C103" s="0" t="n">
+        <f aca="false">A103-1000</f>
+        <v>1026</v>
+      </c>
+      <c r="D103" s="9" t="n">
         <f aca="false">VLOOKUP(A103,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4026</v>
       </c>
-      <c r="D103" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E103" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F103" s="0" t="str">
+      <c r="F103" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G103" s="0" t="str">
         <f aca="false">VLOOKUP(A103,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right rostral anterior cingulate grey matter</v>
       </c>
@@ -8025,17 +8375,21 @@
         <f aca="false">VLOOKUP(A104,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-rostralmiddlefrontal</v>
       </c>
-      <c r="C104" s="9" t="n">
+      <c r="C104" s="0" t="n">
+        <f aca="false">A104-1000</f>
+        <v>1027</v>
+      </c>
+      <c r="D104" s="9" t="n">
         <f aca="false">VLOOKUP(A104,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4027</v>
       </c>
-      <c r="D104" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E104" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F104" s="0" t="str">
+      <c r="F104" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G104" s="0" t="str">
         <f aca="false">VLOOKUP(A104,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right rostral middle frontal grey matter</v>
       </c>
@@ -8048,17 +8402,21 @@
         <f aca="false">VLOOKUP(A105,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-superiorfrontal</v>
       </c>
-      <c r="C105" s="9" t="n">
+      <c r="C105" s="0" t="n">
+        <f aca="false">A105-1000</f>
+        <v>1028</v>
+      </c>
+      <c r="D105" s="9" t="n">
         <f aca="false">VLOOKUP(A105,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4028</v>
       </c>
-      <c r="D105" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E105" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F105" s="0" t="str">
+      <c r="F105" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G105" s="0" t="str">
         <f aca="false">VLOOKUP(A105,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right superior frontal grey matter</v>
       </c>
@@ -8071,17 +8429,21 @@
         <f aca="false">VLOOKUP(A106,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-superiorparietal</v>
       </c>
-      <c r="C106" s="9" t="n">
+      <c r="C106" s="0" t="n">
+        <f aca="false">A106-1000</f>
+        <v>1029</v>
+      </c>
+      <c r="D106" s="9" t="n">
         <f aca="false">VLOOKUP(A106,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4029</v>
       </c>
-      <c r="D106" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E106" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F106" s="0" t="str">
+      <c r="F106" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G106" s="0" t="str">
         <f aca="false">VLOOKUP(A106,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right superior parietal grey matter</v>
       </c>
@@ -8094,17 +8456,21 @@
         <f aca="false">VLOOKUP(A107,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-superiortemporal</v>
       </c>
-      <c r="C107" s="9" t="n">
+      <c r="C107" s="0" t="n">
+        <f aca="false">A107-1000</f>
+        <v>1030</v>
+      </c>
+      <c r="D107" s="9" t="n">
         <f aca="false">VLOOKUP(A107,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4030</v>
       </c>
-      <c r="D107" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E107" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F107" s="0" t="str">
+      <c r="F107" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G107" s="0" t="str">
         <f aca="false">VLOOKUP(A107,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right superior temporal grey matter</v>
       </c>
@@ -8117,17 +8483,21 @@
         <f aca="false">VLOOKUP(A108,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-supramarginal</v>
       </c>
-      <c r="C108" s="9" t="n">
+      <c r="C108" s="0" t="n">
+        <f aca="false">A108-1000</f>
+        <v>1031</v>
+      </c>
+      <c r="D108" s="9" t="n">
         <f aca="false">VLOOKUP(A108,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4031</v>
       </c>
-      <c r="D108" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E108" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F108" s="0" t="str">
+      <c r="F108" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G108" s="0" t="str">
         <f aca="false">VLOOKUP(A108,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right supramarginal grey matter</v>
       </c>
@@ -8140,17 +8510,21 @@
         <f aca="false">VLOOKUP(A109,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-frontalpole</v>
       </c>
-      <c r="C109" s="9" t="n">
+      <c r="C109" s="0" t="n">
+        <f aca="false">A109-1000</f>
+        <v>1032</v>
+      </c>
+      <c r="D109" s="9" t="n">
         <f aca="false">VLOOKUP(A109,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4032</v>
       </c>
-      <c r="D109" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E109" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F109" s="0" t="str">
+      <c r="F109" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G109" s="0" t="str">
         <f aca="false">VLOOKUP(A109,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right frontal pole grey matter</v>
       </c>
@@ -8163,17 +8537,21 @@
         <f aca="false">VLOOKUP(A110,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-temporalpole</v>
       </c>
-      <c r="C110" s="9" t="n">
+      <c r="C110" s="0" t="n">
+        <f aca="false">A110-1000</f>
+        <v>1033</v>
+      </c>
+      <c r="D110" s="9" t="n">
         <f aca="false">VLOOKUP(A110,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4033</v>
       </c>
-      <c r="D110" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E110" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F110" s="0" t="str">
+      <c r="F110" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G110" s="0" t="str">
         <f aca="false">VLOOKUP(A110,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right temporal pole grey matter</v>
       </c>
@@ -8186,17 +8564,21 @@
         <f aca="false">VLOOKUP(A111,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-transversetemporal</v>
       </c>
-      <c r="C111" s="9" t="n">
+      <c r="C111" s="0" t="n">
+        <f aca="false">A111-1000</f>
+        <v>1034</v>
+      </c>
+      <c r="D111" s="9" t="n">
         <f aca="false">VLOOKUP(A111,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4034</v>
       </c>
-      <c r="D111" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E111" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F111" s="0" t="str">
+      <c r="F111" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G111" s="0" t="str">
         <f aca="false">VLOOKUP(A111,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right transverse temporal grey matter</v>
       </c>
@@ -8209,17 +8591,21 @@
         <f aca="false">VLOOKUP(A112,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>ctx-rh-insula</v>
       </c>
-      <c r="C112" s="9" t="n">
+      <c r="C112" s="0" t="n">
+        <f aca="false">A112-1000</f>
+        <v>1035</v>
+      </c>
+      <c r="D112" s="9" t="n">
         <f aca="false">VLOOKUP(A112,'ROI Pair Specification'!$D$3:$H$108,5,0)</f>
         <v>4035</v>
       </c>
-      <c r="D112" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E112" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="F112" s="0" t="str">
+      <c r="F112" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="G112" s="0" t="str">
         <f aca="false">VLOOKUP(A112,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right insula grey matter</v>
       </c>
@@ -8232,17 +8618,21 @@
         <f aca="false">VLOOKUP(A113,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-bankssts</v>
       </c>
-      <c r="C113" s="9" t="n">
+      <c r="C113" s="0" t="n">
+        <f aca="false">A113+1000</f>
+        <v>4001</v>
+      </c>
+      <c r="D113" s="9" t="n">
         <f aca="false">VLOOKUP(A113,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1001</v>
       </c>
-      <c r="D113" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E113" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F113" s="0" t="str">
+      <c r="F113" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G113" s="0" t="str">
         <f aca="false">VLOOKUP(A113,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left banks of superior temporal sulcus white matter</v>
       </c>
@@ -8255,17 +8645,21 @@
         <f aca="false">VLOOKUP(A114,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-caudalanteriorcingulate</v>
       </c>
-      <c r="C114" s="9" t="n">
+      <c r="C114" s="0" t="n">
+        <f aca="false">A114+1000</f>
+        <v>4002</v>
+      </c>
+      <c r="D114" s="9" t="n">
         <f aca="false">VLOOKUP(A114,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1002</v>
       </c>
-      <c r="D114" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E114" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F114" s="0" t="str">
+      <c r="F114" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G114" s="0" t="str">
         <f aca="false">VLOOKUP(A114,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left caudal anterior cingulate white matter</v>
       </c>
@@ -8278,17 +8672,21 @@
         <f aca="false">VLOOKUP(A115,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-caudalmiddlefrontal</v>
       </c>
-      <c r="C115" s="9" t="n">
+      <c r="C115" s="0" t="n">
+        <f aca="false">A115+1000</f>
+        <v>4003</v>
+      </c>
+      <c r="D115" s="9" t="n">
         <f aca="false">VLOOKUP(A115,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1003</v>
       </c>
-      <c r="D115" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E115" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F115" s="0" t="str">
+      <c r="F115" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G115" s="0" t="str">
         <f aca="false">VLOOKUP(A115,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left caudal middle frontal white matter</v>
       </c>
@@ -8301,17 +8699,21 @@
         <f aca="false">VLOOKUP(A116,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-cuneus</v>
       </c>
-      <c r="C116" s="9" t="n">
+      <c r="C116" s="0" t="n">
+        <f aca="false">A116+1000</f>
+        <v>4005</v>
+      </c>
+      <c r="D116" s="9" t="n">
         <f aca="false">VLOOKUP(A116,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1005</v>
       </c>
-      <c r="D116" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E116" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F116" s="0" t="str">
+      <c r="F116" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G116" s="0" t="str">
         <f aca="false">VLOOKUP(A116,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left cuneus white matter</v>
       </c>
@@ -8324,17 +8726,21 @@
         <f aca="false">VLOOKUP(A117,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-entorhinal</v>
       </c>
-      <c r="C117" s="9" t="n">
+      <c r="C117" s="0" t="n">
+        <f aca="false">A117+1000</f>
+        <v>4006</v>
+      </c>
+      <c r="D117" s="9" t="n">
         <f aca="false">VLOOKUP(A117,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1006</v>
       </c>
-      <c r="D117" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E117" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F117" s="0" t="str">
+      <c r="F117" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G117" s="0" t="str">
         <f aca="false">VLOOKUP(A117,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left entorhinal white matter</v>
       </c>
@@ -8347,17 +8753,21 @@
         <f aca="false">VLOOKUP(A118,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-fusiform</v>
       </c>
-      <c r="C118" s="9" t="n">
+      <c r="C118" s="0" t="n">
+        <f aca="false">A118+1000</f>
+        <v>4007</v>
+      </c>
+      <c r="D118" s="9" t="n">
         <f aca="false">VLOOKUP(A118,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1007</v>
       </c>
-      <c r="D118" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E118" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F118" s="0" t="str">
+      <c r="F118" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G118" s="0" t="str">
         <f aca="false">VLOOKUP(A118,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left fusiform white matter</v>
       </c>
@@ -8370,17 +8780,21 @@
         <f aca="false">VLOOKUP(A119,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-inferiorparietal</v>
       </c>
-      <c r="C119" s="9" t="n">
+      <c r="C119" s="0" t="n">
+        <f aca="false">A119+1000</f>
+        <v>4008</v>
+      </c>
+      <c r="D119" s="9" t="n">
         <f aca="false">VLOOKUP(A119,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1008</v>
       </c>
-      <c r="D119" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E119" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F119" s="0" t="str">
+      <c r="F119" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G119" s="0" t="str">
         <f aca="false">VLOOKUP(A119,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left inferior parietal white matter</v>
       </c>
@@ -8393,17 +8807,21 @@
         <f aca="false">VLOOKUP(A120,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-inferiortemporal</v>
       </c>
-      <c r="C120" s="9" t="n">
+      <c r="C120" s="0" t="n">
+        <f aca="false">A120+1000</f>
+        <v>4009</v>
+      </c>
+      <c r="D120" s="9" t="n">
         <f aca="false">VLOOKUP(A120,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1009</v>
       </c>
-      <c r="D120" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E120" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F120" s="0" t="str">
+      <c r="F120" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G120" s="0" t="str">
         <f aca="false">VLOOKUP(A120,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left inferior temporal white matter</v>
       </c>
@@ -8416,17 +8834,21 @@
         <f aca="false">VLOOKUP(A121,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-isthmuscingulate</v>
       </c>
-      <c r="C121" s="9" t="n">
+      <c r="C121" s="0" t="n">
+        <f aca="false">A121+1000</f>
+        <v>4010</v>
+      </c>
+      <c r="D121" s="9" t="n">
         <f aca="false">VLOOKUP(A121,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1010</v>
       </c>
-      <c r="D121" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E121" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F121" s="0" t="str">
+      <c r="F121" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G121" s="0" t="str">
         <f aca="false">VLOOKUP(A121,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left isthmus cingulate white matter</v>
       </c>
@@ -8439,17 +8861,21 @@
         <f aca="false">VLOOKUP(A122,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-lateraloccipital</v>
       </c>
-      <c r="C122" s="9" t="n">
+      <c r="C122" s="0" t="n">
+        <f aca="false">A122+1000</f>
+        <v>4011</v>
+      </c>
+      <c r="D122" s="9" t="n">
         <f aca="false">VLOOKUP(A122,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1011</v>
       </c>
-      <c r="D122" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E122" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F122" s="0" t="str">
+      <c r="F122" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G122" s="0" t="str">
         <f aca="false">VLOOKUP(A122,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lateral occipital white matter</v>
       </c>
@@ -8462,17 +8888,21 @@
         <f aca="false">VLOOKUP(A123,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-lateralorbitofrontal</v>
       </c>
-      <c r="C123" s="9" t="n">
+      <c r="C123" s="0" t="n">
+        <f aca="false">A123+1000</f>
+        <v>4012</v>
+      </c>
+      <c r="D123" s="9" t="n">
         <f aca="false">VLOOKUP(A123,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1012</v>
       </c>
-      <c r="D123" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E123" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F123" s="0" t="str">
+      <c r="F123" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G123" s="0" t="str">
         <f aca="false">VLOOKUP(A123,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lateral orbitofrontal white matter</v>
       </c>
@@ -8485,17 +8915,21 @@
         <f aca="false">VLOOKUP(A124,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-lingual</v>
       </c>
-      <c r="C124" s="9" t="n">
+      <c r="C124" s="0" t="n">
+        <f aca="false">A124+1000</f>
+        <v>4013</v>
+      </c>
+      <c r="D124" s="9" t="n">
         <f aca="false">VLOOKUP(A124,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1013</v>
       </c>
-      <c r="D124" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E124" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F124" s="0" t="str">
+      <c r="F124" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G124" s="0" t="str">
         <f aca="false">VLOOKUP(A124,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left lingual white matter</v>
       </c>
@@ -8508,17 +8942,21 @@
         <f aca="false">VLOOKUP(A125,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-medialorbitofrontal</v>
       </c>
-      <c r="C125" s="9" t="n">
+      <c r="C125" s="0" t="n">
+        <f aca="false">A125+1000</f>
+        <v>4014</v>
+      </c>
+      <c r="D125" s="9" t="n">
         <f aca="false">VLOOKUP(A125,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1014</v>
       </c>
-      <c r="D125" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E125" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F125" s="0" t="str">
+      <c r="F125" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G125" s="0" t="str">
         <f aca="false">VLOOKUP(A125,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left medial orbitofrontal white matter</v>
       </c>
@@ -8531,17 +8969,21 @@
         <f aca="false">VLOOKUP(A126,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-middletemporal</v>
       </c>
-      <c r="C126" s="9" t="n">
+      <c r="C126" s="0" t="n">
+        <f aca="false">A126+1000</f>
+        <v>4015</v>
+      </c>
+      <c r="D126" s="9" t="n">
         <f aca="false">VLOOKUP(A126,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1015</v>
       </c>
-      <c r="D126" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E126" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F126" s="0" t="str">
+      <c r="F126" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G126" s="0" t="str">
         <f aca="false">VLOOKUP(A126,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left middle temporal white matter</v>
       </c>
@@ -8554,17 +8996,21 @@
         <f aca="false">VLOOKUP(A127,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-parahippocampal</v>
       </c>
-      <c r="C127" s="9" t="n">
+      <c r="C127" s="0" t="n">
+        <f aca="false">A127+1000</f>
+        <v>4016</v>
+      </c>
+      <c r="D127" s="9" t="n">
         <f aca="false">VLOOKUP(A127,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1016</v>
       </c>
-      <c r="D127" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E127" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F127" s="0" t="str">
+      <c r="F127" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G127" s="0" t="str">
         <f aca="false">VLOOKUP(A127,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left parahippocampal white matter</v>
       </c>
@@ -8577,17 +9023,21 @@
         <f aca="false">VLOOKUP(A128,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-paracentral</v>
       </c>
-      <c r="C128" s="9" t="n">
+      <c r="C128" s="0" t="n">
+        <f aca="false">A128+1000</f>
+        <v>4017</v>
+      </c>
+      <c r="D128" s="9" t="n">
         <f aca="false">VLOOKUP(A128,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1017</v>
       </c>
-      <c r="D128" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E128" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F128" s="0" t="str">
+      <c r="F128" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G128" s="0" t="str">
         <f aca="false">VLOOKUP(A128,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left paracentral white matter</v>
       </c>
@@ -8600,17 +9050,21 @@
         <f aca="false">VLOOKUP(A129,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-parsopercularis</v>
       </c>
-      <c r="C129" s="9" t="n">
+      <c r="C129" s="0" t="n">
+        <f aca="false">A129+1000</f>
+        <v>4018</v>
+      </c>
+      <c r="D129" s="9" t="n">
         <f aca="false">VLOOKUP(A129,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1018</v>
       </c>
-      <c r="D129" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E129" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F129" s="0" t="str">
+      <c r="F129" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G129" s="0" t="str">
         <f aca="false">VLOOKUP(A129,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pars opercularis white matter</v>
       </c>
@@ -8623,17 +9077,21 @@
         <f aca="false">VLOOKUP(A130,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-parsorbitalis</v>
       </c>
-      <c r="C130" s="9" t="n">
+      <c r="C130" s="0" t="n">
+        <f aca="false">A130+1000</f>
+        <v>4019</v>
+      </c>
+      <c r="D130" s="9" t="n">
         <f aca="false">VLOOKUP(A130,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1019</v>
       </c>
-      <c r="D130" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E130" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F130" s="0" t="str">
+      <c r="F130" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G130" s="0" t="str">
         <f aca="false">VLOOKUP(A130,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pars orbitalis white matter</v>
       </c>
@@ -8646,17 +9104,21 @@
         <f aca="false">VLOOKUP(A131,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-parstriangularis</v>
       </c>
-      <c r="C131" s="9" t="n">
+      <c r="C131" s="0" t="n">
+        <f aca="false">A131+1000</f>
+        <v>4020</v>
+      </c>
+      <c r="D131" s="9" t="n">
         <f aca="false">VLOOKUP(A131,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1020</v>
       </c>
-      <c r="D131" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E131" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F131" s="0" t="str">
+      <c r="F131" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G131" s="0" t="str">
         <f aca="false">VLOOKUP(A131,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pars triangularis white matter</v>
       </c>
@@ -8669,17 +9131,21 @@
         <f aca="false">VLOOKUP(A132,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-pericalcarine</v>
       </c>
-      <c r="C132" s="9" t="n">
+      <c r="C132" s="0" t="n">
+        <f aca="false">A132+1000</f>
+        <v>4021</v>
+      </c>
+      <c r="D132" s="9" t="n">
         <f aca="false">VLOOKUP(A132,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1021</v>
       </c>
-      <c r="D132" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E132" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F132" s="0" t="str">
+      <c r="F132" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G132" s="0" t="str">
         <f aca="false">VLOOKUP(A132,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left pericalcarine white matter</v>
       </c>
@@ -8692,17 +9158,21 @@
         <f aca="false">VLOOKUP(A133,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-postcentral</v>
       </c>
-      <c r="C133" s="9" t="n">
+      <c r="C133" s="0" t="n">
+        <f aca="false">A133+1000</f>
+        <v>4022</v>
+      </c>
+      <c r="D133" s="9" t="n">
         <f aca="false">VLOOKUP(A133,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1022</v>
       </c>
-      <c r="D133" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E133" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F133" s="0" t="str">
+      <c r="F133" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G133" s="0" t="str">
         <f aca="false">VLOOKUP(A133,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left postcentral white matter</v>
       </c>
@@ -8715,17 +9185,21 @@
         <f aca="false">VLOOKUP(A134,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-posteriorcingulate</v>
       </c>
-      <c r="C134" s="9" t="n">
+      <c r="C134" s="0" t="n">
+        <f aca="false">A134+1000</f>
+        <v>4023</v>
+      </c>
+      <c r="D134" s="9" t="n">
         <f aca="false">VLOOKUP(A134,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1023</v>
       </c>
-      <c r="D134" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E134" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F134" s="0" t="str">
+      <c r="F134" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G134" s="0" t="str">
         <f aca="false">VLOOKUP(A134,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left posterior cingulate white matter</v>
       </c>
@@ -8738,17 +9212,21 @@
         <f aca="false">VLOOKUP(A135,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-precentral</v>
       </c>
-      <c r="C135" s="9" t="n">
+      <c r="C135" s="0" t="n">
+        <f aca="false">A135+1000</f>
+        <v>4024</v>
+      </c>
+      <c r="D135" s="9" t="n">
         <f aca="false">VLOOKUP(A135,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1024</v>
       </c>
-      <c r="D135" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E135" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F135" s="0" t="str">
+      <c r="F135" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G135" s="0" t="str">
         <f aca="false">VLOOKUP(A135,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left precentral white matter</v>
       </c>
@@ -8761,17 +9239,21 @@
         <f aca="false">VLOOKUP(A136,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-precuneus</v>
       </c>
-      <c r="C136" s="9" t="n">
+      <c r="C136" s="0" t="n">
+        <f aca="false">A136+1000</f>
+        <v>4025</v>
+      </c>
+      <c r="D136" s="9" t="n">
         <f aca="false">VLOOKUP(A136,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1025</v>
       </c>
-      <c r="D136" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E136" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F136" s="0" t="str">
+      <c r="F136" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G136" s="0" t="str">
         <f aca="false">VLOOKUP(A136,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left precuneus white matter</v>
       </c>
@@ -8784,17 +9266,21 @@
         <f aca="false">VLOOKUP(A137,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-rostralanteriorcingulate</v>
       </c>
-      <c r="C137" s="9" t="n">
+      <c r="C137" s="0" t="n">
+        <f aca="false">A137+1000</f>
+        <v>4026</v>
+      </c>
+      <c r="D137" s="9" t="n">
         <f aca="false">VLOOKUP(A137,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1026</v>
       </c>
-      <c r="D137" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E137" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F137" s="0" t="str">
+      <c r="F137" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G137" s="0" t="str">
         <f aca="false">VLOOKUP(A137,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left rostral anterior cingulate white matter</v>
       </c>
@@ -8807,17 +9293,21 @@
         <f aca="false">VLOOKUP(A138,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-rostralmiddlefrontal</v>
       </c>
-      <c r="C138" s="9" t="n">
+      <c r="C138" s="0" t="n">
+        <f aca="false">A138+1000</f>
+        <v>4027</v>
+      </c>
+      <c r="D138" s="9" t="n">
         <f aca="false">VLOOKUP(A138,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1027</v>
       </c>
-      <c r="D138" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E138" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F138" s="0" t="str">
+      <c r="F138" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G138" s="0" t="str">
         <f aca="false">VLOOKUP(A138,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left rostral middle frontal white matter</v>
       </c>
@@ -8830,17 +9320,21 @@
         <f aca="false">VLOOKUP(A139,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-superiorfrontal</v>
       </c>
-      <c r="C139" s="9" t="n">
+      <c r="C139" s="0" t="n">
+        <f aca="false">A139+1000</f>
+        <v>4028</v>
+      </c>
+      <c r="D139" s="9" t="n">
         <f aca="false">VLOOKUP(A139,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1028</v>
       </c>
-      <c r="D139" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E139" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F139" s="0" t="str">
+      <c r="F139" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G139" s="0" t="str">
         <f aca="false">VLOOKUP(A139,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left superior frontal white matter</v>
       </c>
@@ -8853,17 +9347,21 @@
         <f aca="false">VLOOKUP(A140,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-superiorparietal</v>
       </c>
-      <c r="C140" s="9" t="n">
+      <c r="C140" s="0" t="n">
+        <f aca="false">A140+1000</f>
+        <v>4029</v>
+      </c>
+      <c r="D140" s="9" t="n">
         <f aca="false">VLOOKUP(A140,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1029</v>
       </c>
-      <c r="D140" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E140" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F140" s="0" t="str">
+      <c r="F140" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G140" s="0" t="str">
         <f aca="false">VLOOKUP(A140,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left superior parietal white matter</v>
       </c>
@@ -8876,17 +9374,21 @@
         <f aca="false">VLOOKUP(A141,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-superiortemporal</v>
       </c>
-      <c r="C141" s="9" t="n">
+      <c r="C141" s="0" t="n">
+        <f aca="false">A141+1000</f>
+        <v>4030</v>
+      </c>
+      <c r="D141" s="9" t="n">
         <f aca="false">VLOOKUP(A141,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1030</v>
       </c>
-      <c r="D141" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E141" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F141" s="0" t="str">
+      <c r="F141" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G141" s="0" t="str">
         <f aca="false">VLOOKUP(A141,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left suprior temporal white matter</v>
       </c>
@@ -8899,17 +9401,21 @@
         <f aca="false">VLOOKUP(A142,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-supramarginal</v>
       </c>
-      <c r="C142" s="9" t="n">
+      <c r="C142" s="0" t="n">
+        <f aca="false">A142+1000</f>
+        <v>4031</v>
+      </c>
+      <c r="D142" s="9" t="n">
         <f aca="false">VLOOKUP(A142,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1031</v>
       </c>
-      <c r="D142" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E142" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F142" s="0" t="str">
+      <c r="F142" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G142" s="0" t="str">
         <f aca="false">VLOOKUP(A142,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left supramarginal white matter</v>
       </c>
@@ -8922,17 +9428,21 @@
         <f aca="false">VLOOKUP(A143,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-frontalpole</v>
       </c>
-      <c r="C143" s="9" t="n">
+      <c r="C143" s="0" t="n">
+        <f aca="false">A143+1000</f>
+        <v>4032</v>
+      </c>
+      <c r="D143" s="9" t="n">
         <f aca="false">VLOOKUP(A143,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1032</v>
       </c>
-      <c r="D143" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E143" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F143" s="0" t="str">
+      <c r="F143" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G143" s="0" t="str">
         <f aca="false">VLOOKUP(A143,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left frontal pole white matter</v>
       </c>
@@ -8945,17 +9455,21 @@
         <f aca="false">VLOOKUP(A144,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-temporalpole</v>
       </c>
-      <c r="C144" s="9" t="n">
+      <c r="C144" s="0" t="n">
+        <f aca="false">A144+1000</f>
+        <v>4033</v>
+      </c>
+      <c r="D144" s="9" t="n">
         <f aca="false">VLOOKUP(A144,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1033</v>
       </c>
-      <c r="D144" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E144" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F144" s="0" t="str">
+      <c r="F144" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G144" s="0" t="str">
         <f aca="false">VLOOKUP(A144,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left temporal pole white matter</v>
       </c>
@@ -8968,17 +9482,21 @@
         <f aca="false">VLOOKUP(A145,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-transversetemporal</v>
       </c>
-      <c r="C145" s="9" t="n">
+      <c r="C145" s="0" t="n">
+        <f aca="false">A145+1000</f>
+        <v>4034</v>
+      </c>
+      <c r="D145" s="9" t="n">
         <f aca="false">VLOOKUP(A145,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1034</v>
       </c>
-      <c r="D145" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E145" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F145" s="0" t="str">
+      <c r="F145" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G145" s="0" t="str">
         <f aca="false">VLOOKUP(A145,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left transverse temporal white matter</v>
       </c>
@@ -8991,17 +9509,21 @@
         <f aca="false">VLOOKUP(A146,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-lh-insula</v>
       </c>
-      <c r="C146" s="9" t="n">
+      <c r="C146" s="0" t="n">
+        <f aca="false">A146+1000</f>
+        <v>4035</v>
+      </c>
+      <c r="D146" s="9" t="n">
         <f aca="false">VLOOKUP(A146,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>1035</v>
       </c>
-      <c r="D146" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E146" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F146" s="0" t="str">
+      <c r="F146" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G146" s="0" t="str">
         <f aca="false">VLOOKUP(A146,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left insula white matter</v>
       </c>
@@ -9014,17 +9536,21 @@
         <f aca="false">VLOOKUP(A147,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-bankssts</v>
       </c>
-      <c r="C147" s="9" t="n">
+      <c r="C147" s="0" t="n">
+        <f aca="false">A147-1000</f>
+        <v>3001</v>
+      </c>
+      <c r="D147" s="9" t="n">
         <f aca="false">VLOOKUP(A147,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2001</v>
       </c>
-      <c r="D147" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E147" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F147" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F147" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G147" s="0" t="str">
         <f aca="false">VLOOKUP(A147,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right banks of superior temporal sulcus white matter</v>
       </c>
@@ -9037,17 +9563,21 @@
         <f aca="false">VLOOKUP(A148,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-caudalanteriorcingulate</v>
       </c>
-      <c r="C148" s="9" t="n">
+      <c r="C148" s="0" t="n">
+        <f aca="false">A148-1000</f>
+        <v>3002</v>
+      </c>
+      <c r="D148" s="9" t="n">
         <f aca="false">VLOOKUP(A148,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2002</v>
       </c>
-      <c r="D148" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E148" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F148" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F148" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G148" s="0" t="str">
         <f aca="false">VLOOKUP(A148,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right caudal anterior cingulate white matter</v>
       </c>
@@ -9060,17 +9590,21 @@
         <f aca="false">VLOOKUP(A149,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-caudalmiddlefrontal</v>
       </c>
-      <c r="C149" s="9" t="n">
+      <c r="C149" s="0" t="n">
+        <f aca="false">A149-1000</f>
+        <v>3003</v>
+      </c>
+      <c r="D149" s="9" t="n">
         <f aca="false">VLOOKUP(A149,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2003</v>
       </c>
-      <c r="D149" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E149" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F149" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F149" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G149" s="0" t="str">
         <f aca="false">VLOOKUP(A149,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right caudal middle frontal white matter</v>
       </c>
@@ -9083,17 +9617,21 @@
         <f aca="false">VLOOKUP(A150,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-cuneus</v>
       </c>
-      <c r="C150" s="9" t="n">
+      <c r="C150" s="0" t="n">
+        <f aca="false">A150-1000</f>
+        <v>3005</v>
+      </c>
+      <c r="D150" s="9" t="n">
         <f aca="false">VLOOKUP(A150,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2005</v>
       </c>
-      <c r="D150" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E150" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F150" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F150" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G150" s="0" t="str">
         <f aca="false">VLOOKUP(A150,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right cuneus white matter</v>
       </c>
@@ -9106,17 +9644,21 @@
         <f aca="false">VLOOKUP(A151,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-entorhinal</v>
       </c>
-      <c r="C151" s="9" t="n">
+      <c r="C151" s="0" t="n">
+        <f aca="false">A151-1000</f>
+        <v>3006</v>
+      </c>
+      <c r="D151" s="9" t="n">
         <f aca="false">VLOOKUP(A151,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2006</v>
       </c>
-      <c r="D151" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E151" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F151" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F151" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G151" s="0" t="str">
         <f aca="false">VLOOKUP(A151,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right entorhinal white matter</v>
       </c>
@@ -9129,17 +9671,21 @@
         <f aca="false">VLOOKUP(A152,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-fusiform</v>
       </c>
-      <c r="C152" s="9" t="n">
+      <c r="C152" s="0" t="n">
+        <f aca="false">A152-1000</f>
+        <v>3007</v>
+      </c>
+      <c r="D152" s="9" t="n">
         <f aca="false">VLOOKUP(A152,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2007</v>
       </c>
-      <c r="D152" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E152" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F152" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F152" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G152" s="0" t="str">
         <f aca="false">VLOOKUP(A152,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right fusiform white matter</v>
       </c>
@@ -9152,17 +9698,21 @@
         <f aca="false">VLOOKUP(A153,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-inferiorparietal</v>
       </c>
-      <c r="C153" s="9" t="n">
+      <c r="C153" s="0" t="n">
+        <f aca="false">A153-1000</f>
+        <v>3008</v>
+      </c>
+      <c r="D153" s="9" t="n">
         <f aca="false">VLOOKUP(A153,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2008</v>
       </c>
-      <c r="D153" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E153" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F153" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F153" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G153" s="0" t="str">
         <f aca="false">VLOOKUP(A153,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right inferior parietal white matter</v>
       </c>
@@ -9175,17 +9725,21 @@
         <f aca="false">VLOOKUP(A154,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-inferiortemporal</v>
       </c>
-      <c r="C154" s="9" t="n">
+      <c r="C154" s="0" t="n">
+        <f aca="false">A154-1000</f>
+        <v>3009</v>
+      </c>
+      <c r="D154" s="9" t="n">
         <f aca="false">VLOOKUP(A154,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2009</v>
       </c>
-      <c r="D154" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E154" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F154" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F154" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G154" s="0" t="str">
         <f aca="false">VLOOKUP(A154,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right inferior temporal white matter</v>
       </c>
@@ -9198,17 +9752,21 @@
         <f aca="false">VLOOKUP(A155,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-isthmuscingulate</v>
       </c>
-      <c r="C155" s="9" t="n">
+      <c r="C155" s="0" t="n">
+        <f aca="false">A155-1000</f>
+        <v>3010</v>
+      </c>
+      <c r="D155" s="9" t="n">
         <f aca="false">VLOOKUP(A155,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2010</v>
       </c>
-      <c r="D155" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E155" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F155" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F155" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G155" s="0" t="str">
         <f aca="false">VLOOKUP(A155,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right isthmus cingulate white matter</v>
       </c>
@@ -9221,17 +9779,21 @@
         <f aca="false">VLOOKUP(A156,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-lateraloccipital</v>
       </c>
-      <c r="C156" s="9" t="n">
+      <c r="C156" s="0" t="n">
+        <f aca="false">A156-1000</f>
+        <v>3011</v>
+      </c>
+      <c r="D156" s="9" t="n">
         <f aca="false">VLOOKUP(A156,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2011</v>
       </c>
-      <c r="D156" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E156" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F156" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F156" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G156" s="0" t="str">
         <f aca="false">VLOOKUP(A156,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lateral occipital white matter</v>
       </c>
@@ -9244,17 +9806,21 @@
         <f aca="false">VLOOKUP(A157,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-lateralorbitofrontal</v>
       </c>
-      <c r="C157" s="9" t="n">
+      <c r="C157" s="0" t="n">
+        <f aca="false">A157-1000</f>
+        <v>3012</v>
+      </c>
+      <c r="D157" s="9" t="n">
         <f aca="false">VLOOKUP(A157,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2012</v>
       </c>
-      <c r="D157" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E157" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F157" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F157" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G157" s="0" t="str">
         <f aca="false">VLOOKUP(A157,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lateral orbitofrontal white matter</v>
       </c>
@@ -9267,17 +9833,21 @@
         <f aca="false">VLOOKUP(A158,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-lingual</v>
       </c>
-      <c r="C158" s="9" t="n">
+      <c r="C158" s="0" t="n">
+        <f aca="false">A158-1000</f>
+        <v>3013</v>
+      </c>
+      <c r="D158" s="9" t="n">
         <f aca="false">VLOOKUP(A158,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2013</v>
       </c>
-      <c r="D158" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E158" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F158" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F158" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G158" s="0" t="str">
         <f aca="false">VLOOKUP(A158,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right lingual white matter</v>
       </c>
@@ -9290,17 +9860,21 @@
         <f aca="false">VLOOKUP(A159,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-medialorbitofrontal</v>
       </c>
-      <c r="C159" s="9" t="n">
+      <c r="C159" s="0" t="n">
+        <f aca="false">A159-1000</f>
+        <v>3014</v>
+      </c>
+      <c r="D159" s="9" t="n">
         <f aca="false">VLOOKUP(A159,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2014</v>
       </c>
-      <c r="D159" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E159" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F159" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F159" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G159" s="0" t="str">
         <f aca="false">VLOOKUP(A159,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right meidal orbitofrontal white matter</v>
       </c>
@@ -9313,17 +9887,21 @@
         <f aca="false">VLOOKUP(A160,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-middletemporal</v>
       </c>
-      <c r="C160" s="9" t="n">
+      <c r="C160" s="0" t="n">
+        <f aca="false">A160-1000</f>
+        <v>3015</v>
+      </c>
+      <c r="D160" s="9" t="n">
         <f aca="false">VLOOKUP(A160,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2015</v>
       </c>
-      <c r="D160" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E160" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F160" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F160" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G160" s="0" t="str">
         <f aca="false">VLOOKUP(A160,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right middle temporal white matter</v>
       </c>
@@ -9336,17 +9914,21 @@
         <f aca="false">VLOOKUP(A161,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-parahippocampal</v>
       </c>
-      <c r="C161" s="9" t="n">
+      <c r="C161" s="0" t="n">
+        <f aca="false">A161-1000</f>
+        <v>3016</v>
+      </c>
+      <c r="D161" s="9" t="n">
         <f aca="false">VLOOKUP(A161,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2016</v>
       </c>
-      <c r="D161" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E161" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F161" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F161" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G161" s="0" t="str">
         <f aca="false">VLOOKUP(A161,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right parahippocampal white matter</v>
       </c>
@@ -9359,17 +9941,21 @@
         <f aca="false">VLOOKUP(A162,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-paracentral</v>
       </c>
-      <c r="C162" s="9" t="n">
+      <c r="C162" s="0" t="n">
+        <f aca="false">A162-1000</f>
+        <v>3017</v>
+      </c>
+      <c r="D162" s="9" t="n">
         <f aca="false">VLOOKUP(A162,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2017</v>
       </c>
-      <c r="D162" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E162" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F162" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F162" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G162" s="0" t="str">
         <f aca="false">VLOOKUP(A162,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right paracentral white matter</v>
       </c>
@@ -9382,17 +9968,21 @@
         <f aca="false">VLOOKUP(A163,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-parsopercularis</v>
       </c>
-      <c r="C163" s="9" t="n">
+      <c r="C163" s="0" t="n">
+        <f aca="false">A163-1000</f>
+        <v>3018</v>
+      </c>
+      <c r="D163" s="9" t="n">
         <f aca="false">VLOOKUP(A163,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2018</v>
       </c>
-      <c r="D163" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E163" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F163" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F163" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G163" s="0" t="str">
         <f aca="false">VLOOKUP(A163,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pars opercularis white matter</v>
       </c>
@@ -9405,17 +9995,21 @@
         <f aca="false">VLOOKUP(A164,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-parsorbitalis</v>
       </c>
-      <c r="C164" s="9" t="n">
+      <c r="C164" s="0" t="n">
+        <f aca="false">A164-1000</f>
+        <v>3019</v>
+      </c>
+      <c r="D164" s="9" t="n">
         <f aca="false">VLOOKUP(A164,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2019</v>
       </c>
-      <c r="D164" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E164" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F164" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F164" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G164" s="0" t="str">
         <f aca="false">VLOOKUP(A164,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pars orbitalis white matter</v>
       </c>
@@ -9428,17 +10022,21 @@
         <f aca="false">VLOOKUP(A165,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-parstriangularis</v>
       </c>
-      <c r="C165" s="9" t="n">
+      <c r="C165" s="0" t="n">
+        <f aca="false">A165-1000</f>
+        <v>3020</v>
+      </c>
+      <c r="D165" s="9" t="n">
         <f aca="false">VLOOKUP(A165,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2020</v>
       </c>
-      <c r="D165" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E165" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F165" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F165" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G165" s="0" t="str">
         <f aca="false">VLOOKUP(A165,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pars triangularis white matter</v>
       </c>
@@ -9451,17 +10049,21 @@
         <f aca="false">VLOOKUP(A166,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-pericalcarine</v>
       </c>
-      <c r="C166" s="9" t="n">
+      <c r="C166" s="0" t="n">
+        <f aca="false">A166-1000</f>
+        <v>3021</v>
+      </c>
+      <c r="D166" s="9" t="n">
         <f aca="false">VLOOKUP(A166,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2021</v>
       </c>
-      <c r="D166" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E166" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F166" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F166" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G166" s="0" t="str">
         <f aca="false">VLOOKUP(A166,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right pericalcarine white matter</v>
       </c>
@@ -9474,17 +10076,21 @@
         <f aca="false">VLOOKUP(A167,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-postcentral</v>
       </c>
-      <c r="C167" s="9" t="n">
+      <c r="C167" s="0" t="n">
+        <f aca="false">A167-1000</f>
+        <v>3022</v>
+      </c>
+      <c r="D167" s="9" t="n">
         <f aca="false">VLOOKUP(A167,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2022</v>
       </c>
-      <c r="D167" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E167" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F167" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F167" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G167" s="0" t="str">
         <f aca="false">VLOOKUP(A167,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right postcentral white matter</v>
       </c>
@@ -9497,17 +10103,21 @@
         <f aca="false">VLOOKUP(A168,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-posteriorcingulate</v>
       </c>
-      <c r="C168" s="9" t="n">
+      <c r="C168" s="0" t="n">
+        <f aca="false">A168-1000</f>
+        <v>3023</v>
+      </c>
+      <c r="D168" s="9" t="n">
         <f aca="false">VLOOKUP(A168,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2023</v>
       </c>
-      <c r="D168" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E168" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F168" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F168" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G168" s="0" t="str">
         <f aca="false">VLOOKUP(A168,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right posterior cingulate white matter</v>
       </c>
@@ -9520,17 +10130,21 @@
         <f aca="false">VLOOKUP(A169,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-precentral</v>
       </c>
-      <c r="C169" s="9" t="n">
+      <c r="C169" s="0" t="n">
+        <f aca="false">A169-1000</f>
+        <v>3024</v>
+      </c>
+      <c r="D169" s="9" t="n">
         <f aca="false">VLOOKUP(A169,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2024</v>
       </c>
-      <c r="D169" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E169" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F169" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F169" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G169" s="0" t="str">
         <f aca="false">VLOOKUP(A169,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right precentral white matter</v>
       </c>
@@ -9543,17 +10157,21 @@
         <f aca="false">VLOOKUP(A170,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-precuneus</v>
       </c>
-      <c r="C170" s="9" t="n">
+      <c r="C170" s="0" t="n">
+        <f aca="false">A170-1000</f>
+        <v>3025</v>
+      </c>
+      <c r="D170" s="9" t="n">
         <f aca="false">VLOOKUP(A170,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2025</v>
       </c>
-      <c r="D170" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E170" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F170" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F170" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G170" s="0" t="str">
         <f aca="false">VLOOKUP(A170,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right precuneus white matter</v>
       </c>
@@ -9566,17 +10184,21 @@
         <f aca="false">VLOOKUP(A171,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-rostralanteriorcingulate</v>
       </c>
-      <c r="C171" s="9" t="n">
+      <c r="C171" s="0" t="n">
+        <f aca="false">A171-1000</f>
+        <v>3026</v>
+      </c>
+      <c r="D171" s="9" t="n">
         <f aca="false">VLOOKUP(A171,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2026</v>
       </c>
-      <c r="D171" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E171" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F171" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F171" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G171" s="0" t="str">
         <f aca="false">VLOOKUP(A171,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right rostral anterior cingulate white matter</v>
       </c>
@@ -9589,17 +10211,21 @@
         <f aca="false">VLOOKUP(A172,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-rostralmiddlefrontal</v>
       </c>
-      <c r="C172" s="9" t="n">
+      <c r="C172" s="0" t="n">
+        <f aca="false">A172-1000</f>
+        <v>3027</v>
+      </c>
+      <c r="D172" s="9" t="n">
         <f aca="false">VLOOKUP(A172,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2027</v>
       </c>
-      <c r="D172" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E172" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F172" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F172" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G172" s="0" t="str">
         <f aca="false">VLOOKUP(A172,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right rostral middle frontal white matter</v>
       </c>
@@ -9612,17 +10238,21 @@
         <f aca="false">VLOOKUP(A173,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-superiorfrontal</v>
       </c>
-      <c r="C173" s="9" t="n">
+      <c r="C173" s="0" t="n">
+        <f aca="false">A173-1000</f>
+        <v>3028</v>
+      </c>
+      <c r="D173" s="9" t="n">
         <f aca="false">VLOOKUP(A173,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2028</v>
       </c>
-      <c r="D173" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E173" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F173" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F173" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G173" s="0" t="str">
         <f aca="false">VLOOKUP(A173,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right superior frontal white matter</v>
       </c>
@@ -9635,17 +10265,21 @@
         <f aca="false">VLOOKUP(A174,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-superiorparietal</v>
       </c>
-      <c r="C174" s="9" t="n">
+      <c r="C174" s="0" t="n">
+        <f aca="false">A174-1000</f>
+        <v>3029</v>
+      </c>
+      <c r="D174" s="9" t="n">
         <f aca="false">VLOOKUP(A174,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2029</v>
       </c>
-      <c r="D174" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E174" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F174" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F174" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G174" s="0" t="str">
         <f aca="false">VLOOKUP(A174,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right superior parietal white matter</v>
       </c>
@@ -9658,17 +10292,21 @@
         <f aca="false">VLOOKUP(A175,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-superiortemporal</v>
       </c>
-      <c r="C175" s="9" t="n">
+      <c r="C175" s="0" t="n">
+        <f aca="false">A175-1000</f>
+        <v>3030</v>
+      </c>
+      <c r="D175" s="9" t="n">
         <f aca="false">VLOOKUP(A175,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2030</v>
       </c>
-      <c r="D175" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E175" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F175" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F175" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G175" s="0" t="str">
         <f aca="false">VLOOKUP(A175,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right suprior temporal white matter</v>
       </c>
@@ -9681,17 +10319,21 @@
         <f aca="false">VLOOKUP(A176,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-supramarginal</v>
       </c>
-      <c r="C176" s="9" t="n">
+      <c r="C176" s="0" t="n">
+        <f aca="false">A176-1000</f>
+        <v>3031</v>
+      </c>
+      <c r="D176" s="9" t="n">
         <f aca="false">VLOOKUP(A176,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2031</v>
       </c>
-      <c r="D176" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E176" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F176" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F176" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G176" s="0" t="str">
         <f aca="false">VLOOKUP(A176,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right supramarginal white matter</v>
       </c>
@@ -9704,17 +10346,21 @@
         <f aca="false">VLOOKUP(A177,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-frontalpole</v>
       </c>
-      <c r="C177" s="9" t="n">
+      <c r="C177" s="0" t="n">
+        <f aca="false">A177-1000</f>
+        <v>3032</v>
+      </c>
+      <c r="D177" s="9" t="n">
         <f aca="false">VLOOKUP(A177,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2032</v>
       </c>
-      <c r="D177" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E177" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F177" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F177" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G177" s="0" t="str">
         <f aca="false">VLOOKUP(A177,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right frontal pole white matter</v>
       </c>
@@ -9727,17 +10373,21 @@
         <f aca="false">VLOOKUP(A178,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-temporalpole</v>
       </c>
-      <c r="C178" s="9" t="n">
+      <c r="C178" s="0" t="n">
+        <f aca="false">A178-1000</f>
+        <v>3033</v>
+      </c>
+      <c r="D178" s="9" t="n">
         <f aca="false">VLOOKUP(A178,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2033</v>
       </c>
-      <c r="D178" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E178" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F178" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F178" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G178" s="0" t="str">
         <f aca="false">VLOOKUP(A178,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right temporal pole white matter</v>
       </c>
@@ -9750,17 +10400,21 @@
         <f aca="false">VLOOKUP(A179,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-transversetemporal</v>
       </c>
-      <c r="C179" s="9" t="n">
+      <c r="C179" s="0" t="n">
+        <f aca="false">A179-1000</f>
+        <v>3034</v>
+      </c>
+      <c r="D179" s="9" t="n">
         <f aca="false">VLOOKUP(A179,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2034</v>
       </c>
-      <c r="D179" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E179" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F179" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F179" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G179" s="0" t="str">
         <f aca="false">VLOOKUP(A179,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right transverse temporal white matter</v>
       </c>
@@ -9773,17 +10427,21 @@
         <f aca="false">VLOOKUP(A180,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>wm-rh-insula</v>
       </c>
-      <c r="C180" s="9" t="n">
+      <c r="C180" s="0" t="n">
+        <f aca="false">A180-1000</f>
+        <v>3035</v>
+      </c>
+      <c r="D180" s="9" t="n">
         <f aca="false">VLOOKUP(A180,'ROI Pair Specification'!$A$3:$D$116,4,0)</f>
         <v>2035</v>
       </c>
-      <c r="D180" s="0" t="s">
-        <v>399</v>
-      </c>
       <c r="E180" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F180" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F180" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G180" s="0" t="str">
         <f aca="false">VLOOKUP(A180,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right insula white matter</v>
       </c>
@@ -9796,14 +10454,17 @@
         <f aca="false">VLOOKUP(A181,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Left-UnsegmentedWhiteMatter</v>
       </c>
-      <c r="C181" s="9"/>
-      <c r="D181" s="0" t="s">
-        <v>396</v>
-      </c>
+      <c r="C181" s="0" t="n">
+        <v>5002</v>
+      </c>
+      <c r="D181" s="9"/>
       <c r="E181" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F181" s="0" t="str">
+      <c r="F181" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G181" s="0" t="str">
         <f aca="false">VLOOKUP(A181,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>left unsegmented white matter</v>
       </c>
@@ -9816,14 +10477,17 @@
         <f aca="false">VLOOKUP(A182,'Main ROI Listing'!$A$1:$C$188,2,0)</f>
         <v>Right-UnsegmentedWhiteMatter</v>
       </c>
-      <c r="C182" s="9"/>
-      <c r="D182" s="0" t="s">
-        <v>399</v>
-      </c>
+      <c r="C182" s="0" t="n">
+        <v>5001</v>
+      </c>
+      <c r="D182" s="9"/>
       <c r="E182" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="F182" s="0" t="str">
+        <v>400</v>
+      </c>
+      <c r="F182" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="G182" s="0" t="str">
         <f aca="false">VLOOKUP(A182,'Main ROI Listing'!$A$1:$C$188,3,0)</f>
         <v>right unsegmented white matter</v>
       </c>

</xml_diff>